<commit_message>
Añadida función de enviar el resultado al correo y se han escondido las variables sensibles
</commit_message>
<xml_diff>
--- a/output/news.xlsx
+++ b/output/news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,6 +518,40 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>05-11-2024</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>El Gobierno invierte un millón de euros para la mejora del abastecimiento de agua en el norte de Gran Canaria - InfonorteDigital</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://news.google.com/rss/articles/CBMi4wFBVV95cUxOYkNvMmRBd0tBamZONVNxbzdtYy1ZR3l6SWlQTHFaTUI5ajJaZ190bGVaYkRKcWFLV0xQS0owRGdVcFlMSU1qTC1CVFZnWS1UdWlidEZqeDRnTG1yZGNXOXF2NHVBVGU2UzJhNUNTMFhIWTQ2WVFNMWQ5RmVDTWNfRkJ2WVppTWVGaFNZNHFMRnRqNVdWZnZjMWREZlk1RGdRVW9CMW8ySHlVbkwwUERjanhvMF8zdVl3UHloeExUZXJDWi1kZllxR0M2eGJCczNHeFpwRmxkMU9HNXRjQVBPY0R2TQ?oc=5</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>06-11-2024</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>La Feria Internacional Canagua y Energía impulsa un espacio para los encuentros profesionales entre empresas y visitantes - Canarias Noticias</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://news.google.com/rss/articles/CBMiugFBVV95cUxOMXMzRFBiNnRZUmNrY1JrVmN3S24zSjFPVjBEcVIwTEg4czZORnhIZ0ZDVTJnZVl5QlVrT2lMLTQzVUlxeDVQVmtSZVBXX0R1TUZJUjFPcjU0c1BiQV9GOWNPcGFueUEwTGdmakZqZHNEbkJ2YlNoOG9mbHZlUklRX2QyQjBuUUdzeFA1ZmgtaHBDRzNjZVVhUUp5Umtja1B4bGpEMXhYU0NSVDB0TWpHY3RYQnRKaC1nN1E?oc=5</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>